<commit_message>
brand load optimized and UI grey out feature added
</commit_message>
<xml_diff>
--- a/data/templates/EXTERNAL__Trademark_Tool_Data_LCG_2_0.xlsx
+++ b/data/templates/EXTERNAL__Trademark_Tool_Data_LCG_2_0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Trademark Config" sheetId="1" state="visible" r:id="rId3"/>
@@ -939,20 +939,67 @@
     <author>Unknown Author</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">======
-ID#AAABsjToARM
-Abhradip Choudhuri    (2025-10-20 12:39:21)
-please use ALL if a certain brand+expression is available in all regions, for rest use the country code reference added here and add them like eg: US,UK,CA,AB etc there should be no spaces after the comma
-1 total reaction
-Ilaria Ciavarella reacted with 👍 at 2025-10-20 13:00 PM</t>
+ID#AAABsjToAQE
+    (2025-10-20 12:39:21)
+Brand Names are the actual names that will be returned when the user generates the legal copy. If there is a comma, this single Display Name will be treated as 2 in the trademark</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">======
+ID#AAABsjToAPw
+    (2025-10-20 12:39:21)
+Entity Names are the entities associated with the brand in Columns A and B.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">======
+ID#AAABsjToARc
+    (2025-10-20 12:39:21)
+Entity is Brand - This column was created for brands within JDFOB that are not registered trademarks. For example, Single Barrel is not a registered trademark, but we still want to provide a trademark for users to use. As a result, this returns "[Entity Name] is a registered trademark..."</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">======
+ID#AAABsjToAPg
+    (2025-10-20 12:39:21)
+Third Party - this column was created specifically for third party trademarks within our brands. As of now, Sinatra Century and Select are the only brands where this is applicable.</t>
         </r>
       </text>
     </comment>
@@ -992,7 +1039,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4040" uniqueCount="1644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4045" uniqueCount="1643">
   <si>
     <t xml:space="preserve">Display Names</t>
   </si>
@@ -9788,9 +9835,6 @@
     <t xml:space="preserve">Available Countries</t>
   </si>
   <si>
-    <t xml:space="preserve">ilara please read comment</t>
-  </si>
-  <si>
     <t xml:space="preserve">ALL</t>
   </si>
   <si>
@@ -9870,7 +9914,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -10040,6 +10084,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -10140,7 +10190,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -10353,6 +10403,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10362,7 +10416,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -10406,6 +10460,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF0000FF"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -10670,9 +10732,9 @@
   <dimension ref="A1:M244"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14524,7 +14586,7 @@
         <v>1341</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14532,7 +14594,7 @@
         <v>98</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14540,7 +14602,7 @@
         <v>1348</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14548,7 +14610,7 @@
         <v>1352</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14556,7 +14618,7 @@
         <v>1356</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14564,7 +14626,7 @@
         <v>1360</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14572,7 +14634,7 @@
         <v>1361</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14580,7 +14642,7 @@
         <v>1362</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14588,7 +14650,7 @@
         <v>1364</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14596,7 +14658,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14604,7 +14666,7 @@
         <v>93</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14612,7 +14674,7 @@
         <v>1368</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14620,7 +14682,7 @@
         <v>1372</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14628,7 +14690,7 @@
         <v>1376</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14636,7 +14698,7 @@
         <v>1380</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14644,7 +14706,7 @@
         <v>1384</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14652,7 +14714,7 @@
         <v>1385</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14660,7 +14722,7 @@
         <v>1389</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14668,7 +14730,7 @@
         <v>1392</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14676,7 +14738,7 @@
         <v>1395</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14684,7 +14746,7 @@
         <v>1399</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14692,7 +14754,7 @@
         <v>1403</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14700,7 +14762,7 @@
         <v>1406</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14708,7 +14770,7 @@
         <v>1410</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14716,7 +14778,7 @@
         <v>1414</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14724,7 +14786,7 @@
         <v>1418</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14732,7 +14794,7 @@
         <v>111</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14740,7 +14802,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14748,7 +14810,7 @@
         <v>1429</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14756,7 +14818,7 @@
         <v>1433</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14764,7 +14826,7 @@
         <v>1437</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14772,7 +14834,7 @@
         <v>1441</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14780,7 +14842,7 @@
         <v>1445</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14788,7 +14850,7 @@
         <v>1449</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14796,7 +14858,7 @@
         <v>1452</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14804,7 +14866,7 @@
         <v>1456</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14812,7 +14874,7 @@
         <v>1460</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14820,7 +14882,7 @@
         <v>1461</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14828,7 +14890,7 @@
         <v>1462</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14836,23 +14898,23 @@
         <v>1466</v>
       </c>
       <c r="B40" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="52" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="B41" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="52" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="B42" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14860,7 +14922,7 @@
         <v>79</v>
       </c>
       <c r="B43" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14868,7 +14930,7 @@
         <v>82</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14876,7 +14938,7 @@
         <v>76</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14884,7 +14946,7 @@
         <v>130</v>
       </c>
       <c r="B46" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14892,7 +14954,7 @@
         <v>1478</v>
       </c>
       <c r="B47" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14900,7 +14962,7 @@
         <v>122</v>
       </c>
       <c r="B48" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14908,7 +14970,7 @@
         <v>1485</v>
       </c>
       <c r="B49" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14916,7 +14978,7 @@
         <v>1489</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14924,7 +14986,7 @@
         <v>124</v>
       </c>
       <c r="B51" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14932,7 +14994,7 @@
         <v>1496</v>
       </c>
       <c r="B52" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14940,7 +15002,7 @@
         <v>1500</v>
       </c>
       <c r="B53" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14948,7 +15010,7 @@
         <v>1504</v>
       </c>
       <c r="B54" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14956,7 +15018,7 @@
         <v>1508</v>
       </c>
       <c r="B55" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14964,7 +15026,7 @@
         <v>1512</v>
       </c>
       <c r="B56" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14972,7 +15034,7 @@
         <v>1516</v>
       </c>
       <c r="B57" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14980,7 +15042,7 @@
         <v>1519</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14988,7 +15050,7 @@
         <v>60</v>
       </c>
       <c r="B59" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14996,7 +15058,7 @@
         <v>53</v>
       </c>
       <c r="B60" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15004,7 +15066,7 @@
         <v>1528</v>
       </c>
       <c r="B61" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15012,7 +15074,7 @@
         <v>1532</v>
       </c>
       <c r="B62" s="34" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15020,7 +15082,7 @@
         <v>88</v>
       </c>
       <c r="B63" s="34" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15028,7 +15090,7 @@
         <v>1539</v>
       </c>
       <c r="B64" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15036,7 +15098,7 @@
         <v>1543</v>
       </c>
       <c r="B65" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15044,7 +15106,7 @@
         <v>1547</v>
       </c>
       <c r="B66" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15052,7 +15114,7 @@
         <v>1551</v>
       </c>
       <c r="B67" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15060,7 +15122,7 @@
         <v>1555</v>
       </c>
       <c r="B68" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15068,7 +15130,7 @@
         <v>1559</v>
       </c>
       <c r="B69" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15076,7 +15138,7 @@
         <v>1560</v>
       </c>
       <c r="B70" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15084,7 +15146,7 @@
         <v>1564</v>
       </c>
       <c r="B71" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15092,7 +15154,7 @@
         <v>1568</v>
       </c>
       <c r="B72" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15100,7 +15162,7 @@
         <v>1572</v>
       </c>
       <c r="B73" s="34" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15108,7 +15170,7 @@
         <v>1576</v>
       </c>
       <c r="B74" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15116,7 +15178,7 @@
         <v>1580</v>
       </c>
       <c r="B75" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15124,7 +15186,7 @@
         <v>1584</v>
       </c>
       <c r="B76" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15132,7 +15194,7 @@
         <v>1588</v>
       </c>
       <c r="B77" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15140,7 +15202,7 @@
         <v>1589</v>
       </c>
       <c r="B78" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15148,7 +15210,7 @@
         <v>1593</v>
       </c>
       <c r="B79" s="34" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15156,7 +15218,7 @@
         <v>1594</v>
       </c>
       <c r="B80" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15164,7 +15226,7 @@
         <v>1598</v>
       </c>
       <c r="B81" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15172,7 +15234,7 @@
         <v>1602</v>
       </c>
       <c r="B82" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15180,7 +15242,7 @@
         <v>1604</v>
       </c>
       <c r="B83" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15188,7 +15250,7 @@
         <v>1608</v>
       </c>
       <c r="B84" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15196,7 +15258,7 @@
         <v>1612</v>
       </c>
       <c r="B85" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15204,7 +15266,7 @@
         <v>1614</v>
       </c>
       <c r="B86" s="34" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
   </sheetData>
@@ -15230,7 +15292,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21070,7 +21132,7 @@
   </sheetPr>
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
@@ -39828,16 +39890,19 @@
   </sheetPr>
   <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B67" activeCellId="0" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="91.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="1" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="8.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.75"/>
@@ -39851,6 +39916,18 @@
       <c r="B1" s="41" t="s">
         <v>1618</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="I1" s="2" t="s">
         <v>941</v>
       </c>
@@ -39869,7 +39946,7 @@
         <v>1165</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>1619</v>
+        <v>42</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>944</v>
@@ -39890,7 +39967,10 @@
         <v>98</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>99</v>
       </c>
       <c r="I3" s="42" t="s">
         <v>947</v>
@@ -39911,7 +39991,7 @@
         <v>1348</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I4" s="42" t="s">
         <v>950</v>
@@ -39932,7 +40012,7 @@
         <v>1352</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I5" s="43" t="s">
         <v>952</v>
@@ -39953,7 +40033,7 @@
         <v>1356</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I6" s="44" t="s">
         <v>954</v>
@@ -39974,7 +40054,7 @@
         <v>1360</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>957</v>
@@ -39995,7 +40075,7 @@
         <v>1361</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I8" s="44" t="s">
         <v>959</v>
@@ -40016,7 +40096,7 @@
         <v>1362</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>961</v>
@@ -40034,10 +40114,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="41" t="s">
+        <v>1621</v>
+      </c>
+      <c r="B10" s="41" t="s">
         <v>1622</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>1623</v>
       </c>
       <c r="I10" s="13" t="s">
         <v>964</v>
@@ -40058,7 +40138,7 @@
         <v>1364</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I11" s="43" t="s">
         <v>966</v>
@@ -40079,7 +40159,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I12" s="43" t="s">
         <v>968</v>
@@ -40100,7 +40180,7 @@
         <v>93</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I13" s="13" t="s">
         <v>970</v>
@@ -40121,7 +40201,7 @@
         <v>1368</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I14" s="13" t="s">
         <v>973</v>
@@ -40142,7 +40222,7 @@
         <v>1372</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I15" s="13" t="s">
         <v>975</v>
@@ -40163,7 +40243,7 @@
         <v>1376</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I16" s="43" t="s">
         <v>977</v>
@@ -40184,7 +40264,7 @@
         <v>1380</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I17" s="42" t="s">
         <v>979</v>
@@ -40205,7 +40285,7 @@
         <v>1384</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I18" s="43" t="s">
         <v>981</v>
@@ -40226,7 +40306,7 @@
         <v>1385</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I19" s="13" t="s">
         <v>983</v>
@@ -40247,7 +40327,7 @@
         <v>1389</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I20" s="13" t="s">
         <v>985</v>
@@ -40268,7 +40348,7 @@
         <v>1392</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I21" s="43" t="s">
         <v>988</v>
@@ -40288,8 +40368,8 @@
       <c r="A22" s="41" t="s">
         <v>1395</v>
       </c>
-      <c r="B22" s="41" t="s">
-        <v>1624</v>
+      <c r="B22" s="52" t="s">
+        <v>1623</v>
       </c>
       <c r="I22" s="13" t="s">
         <v>991</v>
@@ -40310,7 +40390,7 @@
         <v>1399</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I23" s="42" t="s">
         <v>994</v>
@@ -40331,7 +40411,7 @@
         <v>1403</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I24" s="42" t="s">
         <v>996</v>
@@ -40352,7 +40432,7 @@
         <v>1406</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I25" s="44" t="s">
         <v>998</v>
@@ -40373,7 +40453,7 @@
         <v>1410</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I26" s="42" t="s">
         <v>1000</v>
@@ -40394,7 +40474,7 @@
         <v>1414</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I27" s="42" t="s">
         <v>1002</v>
@@ -40415,7 +40495,7 @@
         <v>1418</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="I28" s="42" t="s">
         <v>1004</v>
@@ -40436,7 +40516,7 @@
         <v>111</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I29" s="44" t="s">
         <v>1006</v>
@@ -40457,7 +40537,7 @@
         <v>31</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I30" s="43" t="s">
         <v>1009</v>
@@ -40475,7 +40555,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="41" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="B31" s="41" t="s">
         <v>1069</v>
@@ -40499,7 +40579,7 @@
         <v>1429</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I32" s="42" t="s">
         <v>1014</v>
@@ -40520,7 +40600,7 @@
         <v>1433</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I33" s="42" t="s">
         <v>1016</v>
@@ -40541,7 +40621,7 @@
         <v>1437</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I34" s="44" t="s">
         <v>1018</v>
@@ -40562,7 +40642,7 @@
         <v>1441</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I35" s="13" t="s">
         <v>1020</v>
@@ -40583,7 +40663,7 @@
         <v>1445</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I36" s="43" t="s">
         <v>1022</v>
@@ -40604,7 +40684,7 @@
         <v>1449</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I37" s="13" t="s">
         <v>1024</v>
@@ -40625,7 +40705,7 @@
         <v>1452</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
@@ -40636,7 +40716,7 @@
         <v>1456</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I39" s="13" t="s">
         <v>1026</v>
@@ -40657,7 +40737,7 @@
         <v>1460</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I40" s="13" t="s">
         <v>1028</v>
@@ -40678,7 +40758,7 @@
         <v>1461</v>
       </c>
       <c r="B41" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I41" s="42" t="s">
         <v>1030</v>
@@ -40699,7 +40779,7 @@
         <v>1462</v>
       </c>
       <c r="B42" s="51" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I42" s="43" t="s">
         <v>1032</v>
@@ -40720,7 +40800,7 @@
         <v>1466</v>
       </c>
       <c r="B43" s="51" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I43" s="44" t="s">
         <v>1034</v>
@@ -40738,10 +40818,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="41" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="B44" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I44" s="43" t="s">
         <v>1037</v>
@@ -40759,7 +40839,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="41" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="B45" s="41" t="s">
         <v>1228</v>
@@ -40783,7 +40863,7 @@
         <v>79</v>
       </c>
       <c r="B46" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I46" s="44" t="s">
         <v>1042</v>
@@ -40804,7 +40884,7 @@
         <v>82</v>
       </c>
       <c r="B47" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I47" s="42" t="s">
         <v>1045</v>
@@ -40825,7 +40905,7 @@
         <v>76</v>
       </c>
       <c r="B48" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I48" s="42" t="s">
         <v>1047</v>
@@ -40846,7 +40926,7 @@
         <v>130</v>
       </c>
       <c r="B49" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I49" s="13" t="s">
         <v>1049</v>
@@ -40867,7 +40947,7 @@
         <v>1478</v>
       </c>
       <c r="B50" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I50" s="42" t="s">
         <v>1051</v>
@@ -40888,7 +40968,7 @@
         <v>122</v>
       </c>
       <c r="B51" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I51" s="43" t="s">
         <v>1053</v>
@@ -40909,7 +40989,7 @@
         <v>1485</v>
       </c>
       <c r="B52" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I52" s="13" t="s">
         <v>1055</v>
@@ -40930,7 +41010,7 @@
         <v>1489</v>
       </c>
       <c r="B53" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I53" s="13" t="s">
         <v>1057</v>
@@ -40951,7 +41031,7 @@
         <v>124</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I54" s="44" t="s">
         <v>1060</v>
@@ -40972,7 +41052,7 @@
         <v>1496</v>
       </c>
       <c r="B55" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I55" s="42" t="s">
         <v>1063</v>
@@ -40993,7 +41073,7 @@
         <v>1500</v>
       </c>
       <c r="B56" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I56" s="42" t="s">
         <v>1065</v>
@@ -41014,7 +41094,7 @@
         <v>1504</v>
       </c>
       <c r="B57" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I57" s="13" t="s">
         <v>1067</v>
@@ -41035,7 +41115,7 @@
         <v>1508</v>
       </c>
       <c r="B58" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I58" s="13" t="s">
         <v>1069</v>
@@ -41056,7 +41136,7 @@
         <v>1512</v>
       </c>
       <c r="B59" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I59" s="42" t="s">
         <v>1072</v>
@@ -41077,7 +41157,7 @@
         <v>1516</v>
       </c>
       <c r="B60" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I60" s="13" t="s">
         <v>1075</v>
@@ -41098,7 +41178,7 @@
         <v>1519</v>
       </c>
       <c r="B61" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I61" s="43" t="s">
         <v>1077</v>
@@ -41119,7 +41199,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I62" s="44" t="s">
         <v>1079</v>
@@ -41140,7 +41220,7 @@
         <v>53</v>
       </c>
       <c r="B63" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I63" s="42" t="s">
         <v>1082</v>
@@ -41161,7 +41241,7 @@
         <v>1528</v>
       </c>
       <c r="B64" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I64" s="43" t="s">
         <v>1084</v>
@@ -41182,7 +41262,7 @@
         <v>1532</v>
       </c>
       <c r="B65" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I65" s="43" t="s">
         <v>1086</v>
@@ -41203,7 +41283,7 @@
         <v>88</v>
       </c>
       <c r="B66" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I66" s="43" t="s">
         <v>1088</v>
@@ -41220,11 +41300,11 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="41" t="s">
+      <c r="A67" s="53" t="s">
         <v>1539</v>
       </c>
       <c r="B67" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I67" s="44" t="s">
         <v>1090</v>
@@ -41245,7 +41325,7 @@
         <v>1543</v>
       </c>
       <c r="B68" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I68" s="13" t="s">
         <v>1092</v>
@@ -41266,7 +41346,7 @@
         <v>1547</v>
       </c>
       <c r="B69" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I69" s="13" t="s">
         <v>1094</v>
@@ -41287,7 +41367,7 @@
         <v>1551</v>
       </c>
       <c r="B70" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I70" s="44" t="s">
         <v>1096</v>
@@ -41305,10 +41385,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="51" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="B71" s="51" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I71" s="44" t="s">
         <v>1098</v>
@@ -41326,10 +41406,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="51" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="B72" s="51" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I72" s="43" t="s">
         <v>1100</v>
@@ -41350,7 +41430,7 @@
         <v>1555</v>
       </c>
       <c r="B73" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I73" s="43" t="s">
         <v>1102</v>
@@ -41371,7 +41451,7 @@
         <v>1559</v>
       </c>
       <c r="B74" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I74" s="13" t="s">
         <v>1104</v>
@@ -41392,7 +41472,7 @@
         <v>1560</v>
       </c>
       <c r="B75" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I75" s="44" t="s">
         <v>1107</v>
@@ -41413,7 +41493,7 @@
         <v>1564</v>
       </c>
       <c r="B76" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I76" s="13" t="s">
         <v>1110</v>
@@ -41434,7 +41514,7 @@
         <v>1568</v>
       </c>
       <c r="B77" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I77" s="42" t="s">
         <v>1112</v>
@@ -41455,7 +41535,7 @@
         <v>1572</v>
       </c>
       <c r="B78" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I78" s="43" t="s">
         <v>1114</v>
@@ -41476,7 +41556,7 @@
         <v>1576</v>
       </c>
       <c r="B79" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I79" s="44" t="s">
         <v>1116</v>
@@ -41497,7 +41577,7 @@
         <v>1580</v>
       </c>
       <c r="B80" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I80" s="43" t="s">
         <v>1119</v>
@@ -41518,7 +41598,7 @@
         <v>1584</v>
       </c>
       <c r="B81" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I81" s="13" t="s">
         <v>1121</v>
@@ -41539,7 +41619,7 @@
         <v>1588</v>
       </c>
       <c r="B82" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I82" s="42" t="s">
         <v>1123</v>
@@ -41560,7 +41640,7 @@
         <v>1589</v>
       </c>
       <c r="B83" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I83" s="43" t="s">
         <v>1126</v>
@@ -41581,7 +41661,7 @@
         <v>1593</v>
       </c>
       <c r="B84" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I84" s="44" t="s">
         <v>1128</v>
@@ -41602,7 +41682,7 @@
         <v>1594</v>
       </c>
       <c r="B85" s="41" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="I85" s="13" t="s">
         <v>1130</v>
@@ -41623,7 +41703,7 @@
         <v>1598</v>
       </c>
       <c r="B86" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I86" s="43" t="s">
         <v>1132</v>
@@ -41644,7 +41724,7 @@
         <v>1602</v>
       </c>
       <c r="B87" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I87" s="13" t="s">
         <v>1134</v>
@@ -41665,7 +41745,7 @@
         <v>1604</v>
       </c>
       <c r="B88" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I88" s="42" t="s">
         <v>1136</v>
@@ -41686,7 +41766,7 @@
         <v>1608</v>
       </c>
       <c r="B89" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I89" s="44" t="s">
         <v>1138</v>
@@ -41707,7 +41787,7 @@
         <v>1612</v>
       </c>
       <c r="B90" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I90" s="13" t="s">
         <v>1140</v>
@@ -41728,7 +41808,7 @@
         <v>1614</v>
       </c>
       <c r="B91" s="41" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="I91" s="44" t="s">
         <v>1143</v>
@@ -42733,7 +42813,7 @@
         <v>1287</v>
       </c>
       <c r="K157" s="10" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="L157" s="41" t="str">
         <f aca="false">CONCATENATE(I157,",")</f>

</xml_diff>

<commit_message>
logic updated with new expressions
</commit_message>
<xml_diff>
--- a/data/templates/EXTERNAL__Trademark_Tool_Data_LCG_2_0.xlsx
+++ b/data/templates/EXTERNAL__Trademark_Tool_Data_LCG_2_0.xlsx
@@ -946,7 +946,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">======
 ID#AAABsjToAQE
@@ -962,7 +961,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">======
 ID#AAABsjToAPw
@@ -972,22 +970,6 @@
       </text>
     </comment>
     <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">======
-ID#AAABsjToARc
-    (2025-10-20 12:39:21)
-Entity is Brand - This column was created for brands within JDFOB that are not registered trademarks. For example, Single Barrel is not a registered trademark, but we still want to provide a trademark for users to use. As a result, this returns "[Entity Name] is a registered trademark..."</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1039,7 +1021,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4045" uniqueCount="1643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4226" uniqueCount="1651">
   <si>
     <t xml:space="preserve">Display Names</t>
   </si>
@@ -9856,10 +9838,34 @@
     <t xml:space="preserve">Gentleman Jack (RTDs)</t>
   </si>
   <si>
+    <t xml:space="preserve">Jack Daniel's and The Coca-Cola Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COCA-COLA is a trademark of The Coca-Cola Company.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old No.7, Gentleman Jack, Tennessee Fire, Jack Fire, Tennessee Honey, Jack Honey, Tennessee Apple, Tennessee Rye, Single Barrel, No. 27 Gold, Country Cocktails, Winter Jack, Sinatra Select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old No.7, Gentleman Jack, Single Barrel, No. 27 Gold, Sinatra Select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old No.7, Gentleman Jack, Single Barrel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jack Daniel's Old No.7</t>
   </si>
   <si>
     <t xml:space="preserve">Jack Daniel's Old No.7 Puerto Rico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tennessee Fire, Jack Fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tennessee Honey, Jack Honey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country Cocktails</t>
   </si>
   <si>
     <t xml:space="preserve">Old Forester Family of Brands + Mint Julep</t>
@@ -10190,7 +10196,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -10396,6 +10402,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -14586,7 +14600,7 @@
         <v>1341</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>1631</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14594,7 +14608,7 @@
         <v>98</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14602,7 +14616,7 @@
         <v>1348</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14610,7 +14624,7 @@
         <v>1352</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14618,7 +14632,7 @@
         <v>1356</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14626,7 +14640,7 @@
         <v>1360</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14634,7 +14648,7 @@
         <v>1361</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14642,7 +14656,7 @@
         <v>1362</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14650,7 +14664,7 @@
         <v>1364</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14658,7 +14672,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14666,7 +14680,7 @@
         <v>93</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14674,7 +14688,7 @@
         <v>1368</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>1633</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14682,7 +14696,7 @@
         <v>1372</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>1633</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14690,7 +14704,7 @@
         <v>1376</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>1633</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14698,7 +14712,7 @@
         <v>1380</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>1634</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14706,7 +14720,7 @@
         <v>1384</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>1634</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14714,7 +14728,7 @@
         <v>1385</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>1634</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14722,7 +14736,7 @@
         <v>1389</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>1634</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14730,7 +14744,7 @@
         <v>1392</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>1634</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14738,7 +14752,7 @@
         <v>1395</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>1634</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14746,7 +14760,7 @@
         <v>1399</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>1634</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14754,7 +14768,7 @@
         <v>1403</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>1634</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14762,7 +14776,7 @@
         <v>1406</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>1635</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14770,7 +14784,7 @@
         <v>1410</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>1635</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14778,7 +14792,7 @@
         <v>1414</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>1635</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14786,7 +14800,7 @@
         <v>1418</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>1635</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14794,7 +14808,7 @@
         <v>111</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>1636</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14802,7 +14816,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>1637</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14810,7 +14824,7 @@
         <v>1429</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14818,7 +14832,7 @@
         <v>1433</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14826,7 +14840,7 @@
         <v>1437</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14834,7 +14848,7 @@
         <v>1441</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14842,7 +14856,7 @@
         <v>1445</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14850,7 +14864,7 @@
         <v>1449</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>1638</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14858,7 +14872,7 @@
         <v>1452</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14866,7 +14880,7 @@
         <v>1456</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14874,7 +14888,7 @@
         <v>1460</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14882,7 +14896,7 @@
         <v>1461</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14890,7 +14904,7 @@
         <v>1462</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14898,23 +14912,23 @@
         <v>1466</v>
       </c>
       <c r="B40" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="52" t="s">
-        <v>1626</v>
+      <c r="A41" s="54" t="s">
+        <v>1631</v>
       </c>
       <c r="B41" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="52" t="s">
-        <v>1627</v>
+      <c r="A42" s="54" t="s">
+        <v>1632</v>
       </c>
       <c r="B42" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14922,7 +14936,7 @@
         <v>79</v>
       </c>
       <c r="B43" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14930,7 +14944,7 @@
         <v>82</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14938,7 +14952,7 @@
         <v>76</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14946,7 +14960,7 @@
         <v>130</v>
       </c>
       <c r="B46" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14954,7 +14968,7 @@
         <v>1478</v>
       </c>
       <c r="B47" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14962,7 +14976,7 @@
         <v>122</v>
       </c>
       <c r="B48" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14970,7 +14984,7 @@
         <v>1485</v>
       </c>
       <c r="B49" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14978,7 +14992,7 @@
         <v>1489</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14986,7 +15000,7 @@
         <v>124</v>
       </c>
       <c r="B51" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14994,7 +15008,7 @@
         <v>1496</v>
       </c>
       <c r="B52" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15002,7 +15016,7 @@
         <v>1500</v>
       </c>
       <c r="B53" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15010,7 +15024,7 @@
         <v>1504</v>
       </c>
       <c r="B54" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15018,7 +15032,7 @@
         <v>1508</v>
       </c>
       <c r="B55" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15026,7 +15040,7 @@
         <v>1512</v>
       </c>
       <c r="B56" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15034,7 +15048,7 @@
         <v>1516</v>
       </c>
       <c r="B57" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15042,7 +15056,7 @@
         <v>1519</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15050,7 +15064,7 @@
         <v>60</v>
       </c>
       <c r="B59" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15058,7 +15072,7 @@
         <v>53</v>
       </c>
       <c r="B60" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15066,7 +15080,7 @@
         <v>1528</v>
       </c>
       <c r="B61" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15074,7 +15088,7 @@
         <v>1532</v>
       </c>
       <c r="B62" s="34" t="s">
-        <v>1640</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15082,7 +15096,7 @@
         <v>88</v>
       </c>
       <c r="B63" s="34" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15090,7 +15104,7 @@
         <v>1539</v>
       </c>
       <c r="B64" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15098,7 +15112,7 @@
         <v>1543</v>
       </c>
       <c r="B65" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15106,7 +15120,7 @@
         <v>1547</v>
       </c>
       <c r="B66" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15114,7 +15128,7 @@
         <v>1551</v>
       </c>
       <c r="B67" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15122,7 +15136,7 @@
         <v>1555</v>
       </c>
       <c r="B68" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15130,7 +15144,7 @@
         <v>1559</v>
       </c>
       <c r="B69" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15138,7 +15152,7 @@
         <v>1560</v>
       </c>
       <c r="B70" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15146,7 +15160,7 @@
         <v>1564</v>
       </c>
       <c r="B71" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15154,7 +15168,7 @@
         <v>1568</v>
       </c>
       <c r="B72" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15162,7 +15176,7 @@
         <v>1572</v>
       </c>
       <c r="B73" s="34" t="s">
-        <v>1642</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15170,7 +15184,7 @@
         <v>1576</v>
       </c>
       <c r="B74" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15178,7 +15192,7 @@
         <v>1580</v>
       </c>
       <c r="B75" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15186,7 +15200,7 @@
         <v>1584</v>
       </c>
       <c r="B76" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15194,7 +15208,7 @@
         <v>1588</v>
       </c>
       <c r="B77" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15202,7 +15216,7 @@
         <v>1589</v>
       </c>
       <c r="B78" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15210,7 +15224,7 @@
         <v>1593</v>
       </c>
       <c r="B79" s="34" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15218,7 +15232,7 @@
         <v>1594</v>
       </c>
       <c r="B80" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15226,7 +15240,7 @@
         <v>1598</v>
       </c>
       <c r="B81" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15234,7 +15248,7 @@
         <v>1602</v>
       </c>
       <c r="B82" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15242,7 +15256,7 @@
         <v>1604</v>
       </c>
       <c r="B83" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15250,7 +15264,7 @@
         <v>1608</v>
       </c>
       <c r="B84" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15258,7 +15272,7 @@
         <v>1612</v>
       </c>
       <c r="B85" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15266,7 +15280,7 @@
         <v>1614</v>
       </c>
       <c r="B86" s="34" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
     </row>
   </sheetData>
@@ -39890,16 +39904,16 @@
   </sheetPr>
   <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B67" activeCellId="0" sqref="B67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="50.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="8.63"/>
@@ -39922,12 +39936,10 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="4"/>
       <c r="I1" s="2" t="s">
         <v>941</v>
       </c>
@@ -39945,9 +39957,13 @@
       <c r="B2" s="41" t="s">
         <v>1165</v>
       </c>
-      <c r="C2" s="41" t="s">
-        <v>42</v>
-      </c>
+      <c r="C2" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="53"/>
       <c r="I2" s="13" t="s">
         <v>944</v>
       </c>
@@ -39969,9 +39985,13 @@
       <c r="B3" s="41" t="s">
         <v>1619</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="C3" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="53"/>
       <c r="I3" s="42" t="s">
         <v>947</v>
       </c>
@@ -39993,6 +40013,13 @@
       <c r="B4" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C4" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="53"/>
       <c r="I4" s="42" t="s">
         <v>950</v>
       </c>
@@ -40014,6 +40041,13 @@
       <c r="B5" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C5" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="53"/>
       <c r="I5" s="43" t="s">
         <v>952</v>
       </c>
@@ -40035,6 +40069,13 @@
       <c r="B6" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C6" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="53"/>
       <c r="I6" s="44" t="s">
         <v>954</v>
       </c>
@@ -40056,6 +40097,13 @@
       <c r="B7" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C7" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="53"/>
       <c r="I7" s="13" t="s">
         <v>957</v>
       </c>
@@ -40077,6 +40125,13 @@
       <c r="B8" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C8" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="53"/>
       <c r="I8" s="44" t="s">
         <v>959</v>
       </c>
@@ -40098,6 +40153,13 @@
       <c r="B9" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C9" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="53"/>
       <c r="I9" s="13" t="s">
         <v>961</v>
       </c>
@@ -40119,6 +40181,13 @@
       <c r="B10" s="41" t="s">
         <v>1622</v>
       </c>
+      <c r="C10" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="53"/>
       <c r="I10" s="13" t="s">
         <v>964</v>
       </c>
@@ -40140,6 +40209,13 @@
       <c r="B11" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C11" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="53"/>
       <c r="I11" s="43" t="s">
         <v>966</v>
       </c>
@@ -40161,6 +40237,13 @@
       <c r="B12" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C12" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="53"/>
       <c r="I12" s="43" t="s">
         <v>968</v>
       </c>
@@ -40182,6 +40265,13 @@
       <c r="B13" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C13" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="53"/>
       <c r="I13" s="13" t="s">
         <v>970</v>
       </c>
@@ -40203,6 +40293,13 @@
       <c r="B14" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C14" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="53"/>
       <c r="I14" s="13" t="s">
         <v>973</v>
       </c>
@@ -40224,6 +40321,13 @@
       <c r="B15" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C15" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="53"/>
       <c r="I15" s="13" t="s">
         <v>975</v>
       </c>
@@ -40245,6 +40349,13 @@
       <c r="B16" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C16" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="53"/>
       <c r="I16" s="43" t="s">
         <v>977</v>
       </c>
@@ -40266,6 +40377,13 @@
       <c r="B17" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C17" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" s="53"/>
       <c r="I17" s="42" t="s">
         <v>979</v>
       </c>
@@ -40287,6 +40405,13 @@
       <c r="B18" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C18" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" s="53"/>
       <c r="I18" s="43" t="s">
         <v>981</v>
       </c>
@@ -40308,6 +40433,13 @@
       <c r="B19" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C19" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="E19" s="53"/>
       <c r="I19" s="13" t="s">
         <v>983</v>
       </c>
@@ -40329,6 +40461,13 @@
       <c r="B20" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C20" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" s="53"/>
       <c r="I20" s="13" t="s">
         <v>985</v>
       </c>
@@ -40350,6 +40489,13 @@
       <c r="B21" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C21" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" s="53"/>
       <c r="I21" s="43" t="s">
         <v>988</v>
       </c>
@@ -40368,9 +40514,16 @@
       <c r="A22" s="41" t="s">
         <v>1395</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="54" t="s">
         <v>1623</v>
       </c>
+      <c r="C22" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="E22" s="53"/>
       <c r="I22" s="13" t="s">
         <v>991</v>
       </c>
@@ -40392,6 +40545,13 @@
       <c r="B23" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C23" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" s="53"/>
       <c r="I23" s="42" t="s">
         <v>994</v>
       </c>
@@ -40413,6 +40573,13 @@
       <c r="B24" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C24" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="E24" s="53"/>
       <c r="I24" s="42" t="s">
         <v>996</v>
       </c>
@@ -40434,6 +40601,13 @@
       <c r="B25" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C25" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="53"/>
       <c r="I25" s="44" t="s">
         <v>998</v>
       </c>
@@ -40455,6 +40629,13 @@
       <c r="B26" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C26" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="53"/>
       <c r="I26" s="42" t="s">
         <v>1000</v>
       </c>
@@ -40476,6 +40657,13 @@
       <c r="B27" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C27" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="53"/>
       <c r="I27" s="42" t="s">
         <v>1002</v>
       </c>
@@ -40497,6 +40685,13 @@
       <c r="B28" s="41" t="s">
         <v>1624</v>
       </c>
+      <c r="C28" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="53"/>
       <c r="I28" s="42" t="s">
         <v>1004</v>
       </c>
@@ -40518,6 +40713,13 @@
       <c r="B29" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C29" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="53"/>
       <c r="I29" s="44" t="s">
         <v>1006</v>
       </c>
@@ -40539,6 +40741,13 @@
       <c r="B30" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C30" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="53"/>
       <c r="I30" s="43" t="s">
         <v>1009</v>
       </c>
@@ -40560,6 +40769,13 @@
       <c r="B31" s="41" t="s">
         <v>1069</v>
       </c>
+      <c r="C31" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="53"/>
       <c r="I31" s="44" t="s">
         <v>1011</v>
       </c>
@@ -40581,6 +40797,13 @@
       <c r="B32" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C32" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" s="53"/>
       <c r="I32" s="42" t="s">
         <v>1014</v>
       </c>
@@ -40602,6 +40825,13 @@
       <c r="B33" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C33" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="53"/>
       <c r="I33" s="42" t="s">
         <v>1016</v>
       </c>
@@ -40623,6 +40853,13 @@
       <c r="B34" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C34" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="53"/>
       <c r="I34" s="44" t="s">
         <v>1018</v>
       </c>
@@ -40644,6 +40881,13 @@
       <c r="B35" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C35" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="53"/>
       <c r="I35" s="13" t="s">
         <v>1020</v>
       </c>
@@ -40665,6 +40909,13 @@
       <c r="B36" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C36" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="53"/>
       <c r="I36" s="43" t="s">
         <v>1022</v>
       </c>
@@ -40686,6 +40937,13 @@
       <c r="B37" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C37" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="53"/>
       <c r="I37" s="13" t="s">
         <v>1024</v>
       </c>
@@ -40707,6 +40965,15 @@
       <c r="B38" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C38" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="52" t="s">
+        <v>1626</v>
+      </c>
+      <c r="E38" s="52" t="s">
+        <v>1627</v>
+      </c>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
@@ -40718,6 +40985,13 @@
       <c r="B39" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C39" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" s="53"/>
       <c r="I39" s="13" t="s">
         <v>1026</v>
       </c>
@@ -40739,6 +41013,13 @@
       <c r="B40" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C40" s="52" t="s">
+        <v>1628</v>
+      </c>
+      <c r="D40" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" s="53"/>
       <c r="I40" s="13" t="s">
         <v>1028</v>
       </c>
@@ -40760,6 +41041,13 @@
       <c r="B41" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C41" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41" s="53"/>
       <c r="I41" s="42" t="s">
         <v>1030</v>
       </c>
@@ -40781,6 +41069,13 @@
       <c r="B42" s="51" t="s">
         <v>1620</v>
       </c>
+      <c r="C42" s="52" t="s">
+        <v>1629</v>
+      </c>
+      <c r="D42" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42" s="53"/>
       <c r="I42" s="43" t="s">
         <v>1032</v>
       </c>
@@ -40802,6 +41097,13 @@
       <c r="B43" s="51" t="s">
         <v>1620</v>
       </c>
+      <c r="C43" s="52" t="s">
+        <v>1630</v>
+      </c>
+      <c r="D43" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43" s="53"/>
       <c r="I43" s="44" t="s">
         <v>1034</v>
       </c>
@@ -40818,11 +41120,18 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="41" t="s">
-        <v>1626</v>
+        <v>1631</v>
       </c>
       <c r="B44" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C44" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="53"/>
       <c r="I44" s="43" t="s">
         <v>1037</v>
       </c>
@@ -40839,11 +41148,18 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="41" t="s">
-        <v>1627</v>
+        <v>1632</v>
       </c>
       <c r="B45" s="41" t="s">
         <v>1228</v>
       </c>
+      <c r="C45" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="53"/>
       <c r="I45" s="44" t="s">
         <v>1040</v>
       </c>
@@ -40865,6 +41181,13 @@
       <c r="B46" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C46" s="52" t="s">
+        <v>1633</v>
+      </c>
+      <c r="D46" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="53"/>
       <c r="I46" s="44" t="s">
         <v>1042</v>
       </c>
@@ -40886,6 +41209,13 @@
       <c r="B47" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C47" s="52" t="s">
+        <v>1634</v>
+      </c>
+      <c r="D47" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="53"/>
       <c r="I47" s="42" t="s">
         <v>1045</v>
       </c>
@@ -40907,6 +41237,13 @@
       <c r="B48" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C48" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" s="53"/>
       <c r="I48" s="42" t="s">
         <v>1047</v>
       </c>
@@ -40928,6 +41265,13 @@
       <c r="B49" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C49" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" s="53"/>
       <c r="I49" s="13" t="s">
         <v>1049</v>
       </c>
@@ -40949,6 +41293,13 @@
       <c r="B50" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C50" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50" s="53"/>
       <c r="I50" s="42" t="s">
         <v>1051</v>
       </c>
@@ -40970,6 +41321,13 @@
       <c r="B51" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C51" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" s="53"/>
       <c r="I51" s="43" t="s">
         <v>1053</v>
       </c>
@@ -40991,6 +41349,13 @@
       <c r="B52" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C52" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="53"/>
       <c r="I52" s="13" t="s">
         <v>1055</v>
       </c>
@@ -41012,6 +41377,13 @@
       <c r="B53" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C53" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" s="53"/>
       <c r="I53" s="13" t="s">
         <v>1057</v>
       </c>
@@ -41033,6 +41405,13 @@
       <c r="B54" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C54" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E54" s="53"/>
       <c r="I54" s="44" t="s">
         <v>1060</v>
       </c>
@@ -41054,6 +41433,13 @@
       <c r="B55" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C55" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" s="53"/>
       <c r="I55" s="42" t="s">
         <v>1063</v>
       </c>
@@ -41075,6 +41461,13 @@
       <c r="B56" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C56" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D56" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" s="53"/>
       <c r="I56" s="42" t="s">
         <v>1065</v>
       </c>
@@ -41096,6 +41489,13 @@
       <c r="B57" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C57" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E57" s="53"/>
       <c r="I57" s="13" t="s">
         <v>1067</v>
       </c>
@@ -41117,6 +41517,13 @@
       <c r="B58" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C58" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E58" s="53"/>
       <c r="I58" s="13" t="s">
         <v>1069</v>
       </c>
@@ -41138,6 +41545,13 @@
       <c r="B59" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C59" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D59" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E59" s="53"/>
       <c r="I59" s="42" t="s">
         <v>1072</v>
       </c>
@@ -41159,6 +41573,13 @@
       <c r="B60" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C60" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D60" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E60" s="53"/>
       <c r="I60" s="13" t="s">
         <v>1075</v>
       </c>
@@ -41180,6 +41601,13 @@
       <c r="B61" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C61" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61" s="53"/>
       <c r="I61" s="43" t="s">
         <v>1077</v>
       </c>
@@ -41201,6 +41629,15 @@
       <c r="B62" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C62" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="D62" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E62" s="52" t="s">
+        <v>63</v>
+      </c>
       <c r="I62" s="44" t="s">
         <v>1079</v>
       </c>
@@ -41222,6 +41659,13 @@
       <c r="B63" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C63" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="D63" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E63" s="53"/>
       <c r="I63" s="42" t="s">
         <v>1082</v>
       </c>
@@ -41243,6 +41687,13 @@
       <c r="B64" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C64" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E64" s="53"/>
       <c r="I64" s="43" t="s">
         <v>1084</v>
       </c>
@@ -41264,6 +41715,13 @@
       <c r="B65" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C65" s="52" t="s">
+        <v>1635</v>
+      </c>
+      <c r="D65" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E65" s="53"/>
       <c r="I65" s="43" t="s">
         <v>1086</v>
       </c>
@@ -41285,6 +41743,13 @@
       <c r="B66" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C66" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="D66" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E66" s="53"/>
       <c r="I66" s="43" t="s">
         <v>1088</v>
       </c>
@@ -41300,12 +41765,19 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="53" t="s">
+      <c r="A67" s="55" t="s">
         <v>1539</v>
       </c>
       <c r="B67" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C67" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D67" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E67" s="53"/>
       <c r="I67" s="44" t="s">
         <v>1090</v>
       </c>
@@ -41327,6 +41799,13 @@
       <c r="B68" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C68" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D68" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E68" s="53"/>
       <c r="I68" s="13" t="s">
         <v>1092</v>
       </c>
@@ -41348,6 +41827,13 @@
       <c r="B69" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C69" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D69" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E69" s="53"/>
       <c r="I69" s="13" t="s">
         <v>1094</v>
       </c>
@@ -41369,6 +41855,13 @@
       <c r="B70" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C70" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D70" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E70" s="53"/>
       <c r="I70" s="44" t="s">
         <v>1096</v>
       </c>
@@ -41385,11 +41878,18 @@
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="51" t="s">
-        <v>1628</v>
+        <v>1636</v>
       </c>
       <c r="B71" s="51" t="s">
         <v>1620</v>
       </c>
+      <c r="C71" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D71" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E71" s="53"/>
       <c r="I71" s="44" t="s">
         <v>1098</v>
       </c>
@@ -41406,11 +41906,18 @@
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="51" t="s">
-        <v>1629</v>
+        <v>1637</v>
       </c>
       <c r="B72" s="51" t="s">
         <v>1620</v>
       </c>
+      <c r="C72" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D72" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E72" s="53"/>
       <c r="I72" s="43" t="s">
         <v>1100</v>
       </c>
@@ -41432,6 +41939,13 @@
       <c r="B73" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C73" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D73" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E73" s="53"/>
       <c r="I73" s="43" t="s">
         <v>1102</v>
       </c>
@@ -41453,6 +41967,13 @@
       <c r="B74" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C74" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D74" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E74" s="53"/>
       <c r="I74" s="13" t="s">
         <v>1104</v>
       </c>
@@ -41474,6 +41995,13 @@
       <c r="B75" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C75" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D75" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E75" s="53"/>
       <c r="I75" s="44" t="s">
         <v>1107</v>
       </c>
@@ -41495,6 +42023,13 @@
       <c r="B76" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C76" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D76" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E76" s="53"/>
       <c r="I76" s="13" t="s">
         <v>1110</v>
       </c>
@@ -41516,6 +42051,13 @@
       <c r="B77" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C77" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D77" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E77" s="53"/>
       <c r="I77" s="42" t="s">
         <v>1112</v>
       </c>
@@ -41537,6 +42079,13 @@
       <c r="B78" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C78" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D78" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="E78" s="53"/>
       <c r="I78" s="43" t="s">
         <v>1114</v>
       </c>
@@ -41558,6 +42107,13 @@
       <c r="B79" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C79" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D79" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="53"/>
       <c r="I79" s="44" t="s">
         <v>1116</v>
       </c>
@@ -41579,6 +42135,13 @@
       <c r="B80" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C80" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D80" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" s="53"/>
       <c r="I80" s="43" t="s">
         <v>1119</v>
       </c>
@@ -41600,6 +42163,13 @@
       <c r="B81" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C81" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D81" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" s="53"/>
       <c r="I81" s="13" t="s">
         <v>1121</v>
       </c>
@@ -41621,6 +42191,13 @@
       <c r="B82" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C82" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D82" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="53"/>
       <c r="I82" s="42" t="s">
         <v>1123</v>
       </c>
@@ -41642,6 +42219,13 @@
       <c r="B83" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C83" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D83" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E83" s="53"/>
       <c r="I83" s="43" t="s">
         <v>1126</v>
       </c>
@@ -41663,6 +42247,13 @@
       <c r="B84" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C84" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D84" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E84" s="53"/>
       <c r="I84" s="44" t="s">
         <v>1128</v>
       </c>
@@ -41684,6 +42275,13 @@
       <c r="B85" s="41" t="s">
         <v>1619</v>
       </c>
+      <c r="C85" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D85" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E85" s="53"/>
       <c r="I85" s="13" t="s">
         <v>1130</v>
       </c>
@@ -41705,6 +42303,13 @@
       <c r="B86" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C86" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D86" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E86" s="53"/>
       <c r="I86" s="43" t="s">
         <v>1132</v>
       </c>
@@ -41726,6 +42331,13 @@
       <c r="B87" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C87" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D87" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E87" s="53"/>
       <c r="I87" s="13" t="s">
         <v>1134</v>
       </c>
@@ -41747,6 +42359,13 @@
       <c r="B88" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C88" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D88" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E88" s="53"/>
       <c r="I88" s="42" t="s">
         <v>1136</v>
       </c>
@@ -41768,6 +42387,13 @@
       <c r="B89" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C89" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D89" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E89" s="53"/>
       <c r="I89" s="44" t="s">
         <v>1138</v>
       </c>
@@ -41789,6 +42415,13 @@
       <c r="B90" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C90" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D90" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E90" s="53"/>
       <c r="I90" s="13" t="s">
         <v>1140</v>
       </c>
@@ -41810,6 +42443,13 @@
       <c r="B91" s="41" t="s">
         <v>1620</v>
       </c>
+      <c r="C91" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D91" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E91" s="53"/>
       <c r="I91" s="44" t="s">
         <v>1143</v>
       </c>
@@ -41831,6 +42471,13 @@
       <c r="B92" s="41" t="s">
         <v>1223</v>
       </c>
+      <c r="C92" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="D92" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="E92" s="53"/>
       <c r="I92" s="42" t="s">
         <v>1145</v>
       </c>
@@ -42813,7 +43460,7 @@
         <v>1287</v>
       </c>
       <c r="K157" s="10" t="s">
-        <v>1630</v>
+        <v>1638</v>
       </c>
       <c r="L157" s="41" t="str">
         <f aca="false">CONCATENATE(I157,",")</f>

</xml_diff>

<commit_message>
copygenerator and template services fixed
</commit_message>
<xml_diff>
--- a/data/templates/EXTERNAL__Trademark_Tool_Data_LCG_2_0.xlsx
+++ b/data/templates/EXTERNAL__Trademark_Tool_Data_LCG_2_0.xlsx
@@ -10805,9 +10805,9 @@
   <dimension ref="A1:M244"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="J3" activeCellId="2" sqref="D59 D61 J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14646,7 +14646,7 @@
   <dimension ref="A1:B86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
+      <selection pane="topLeft" activeCell="E47" activeCellId="2" sqref="D59 D61 E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15365,7 +15365,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="C1" activeCellId="2" sqref="D59 D61 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20145,7 +20145,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="D59 D61 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21206,11 +21206,11 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O14" activeCellId="0" sqref="O14"/>
+      <selection pane="bottomRight" activeCell="T6" activeCellId="2" sqref="D59 D61 T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31645,7 +31645,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="2" sqref="D59 D61 A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33473,7 +33473,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D74" activeCellId="0" sqref="D74"/>
+      <selection pane="bottomLeft" activeCell="D74" activeCellId="2" sqref="D59 D61 D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36352,7 +36352,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="D59 D61 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37392,7 +37392,7 @@
   <dimension ref="A1:AC994"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="D61" activeCellId="1" sqref="D59 D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -42029,7 +42029,7 @@
   <dimension ref="A1:L1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="2" sqref="D59 D61 D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>